<commit_message>
fix aluop for lw sw
</commit_message>
<xml_diff>
--- a/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
+++ b/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franky/2023秋硬件综合训练课设资料发布包/cpu21-riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6A187-20EA-A24B-98B9-024E4B4E3EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02981F60-18F5-4D4F-B01C-9938168B6E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2100,8 +2100,8 @@
   </sheetPr>
   <dimension ref="A1:AL62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -3634,22 +3634,24 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="38" t="str">
+      <c r="P16" s="37">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="38">
         <f t="shared" si="8"/>
-        <v>X</v>
-      </c>
-      <c r="R16" s="38" t="str">
+        <v>0</v>
+      </c>
+      <c r="R16" s="38">
         <f t="shared" si="9"/>
-        <v>X</v>
-      </c>
-      <c r="S16" s="38" t="str">
+        <v>1</v>
+      </c>
+      <c r="S16" s="38">
         <f t="shared" si="10"/>
-        <v>X</v>
-      </c>
-      <c r="T16" s="38" t="str">
+        <v>0</v>
+      </c>
+      <c r="T16" s="38">
         <f t="shared" si="11"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="U16" s="30">
         <v>1</v>
@@ -3729,22 +3731,24 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="62" t="str">
+      <c r="P17" s="61">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="62">
         <f t="shared" si="8"/>
-        <v>X</v>
-      </c>
-      <c r="R17" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="R17" s="62">
         <f t="shared" si="9"/>
-        <v>X</v>
-      </c>
-      <c r="S17" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="S17" s="62">
         <f t="shared" si="10"/>
-        <v>X</v>
-      </c>
-      <c r="T17" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="T17" s="62">
         <f t="shared" si="11"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="U17" s="56"/>
       <c r="V17" s="56">
@@ -4748,22 +4752,24 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="38" t="str">
+      <c r="P28" s="37">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="38">
         <f t="shared" si="8"/>
-        <v>X</v>
-      </c>
-      <c r="R28" s="38" t="str">
+        <v>0</v>
+      </c>
+      <c r="R28" s="38">
         <f t="shared" si="9"/>
-        <v>X</v>
-      </c>
-      <c r="S28" s="38" t="str">
+        <v>1</v>
+      </c>
+      <c r="S28" s="38">
         <f t="shared" si="10"/>
-        <v>X</v>
-      </c>
-      <c r="T28" s="38" t="str">
+        <v>0</v>
+      </c>
+      <c r="T28" s="38">
         <f t="shared" si="11"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="U28" s="30"/>
       <c r="V28" s="30">
@@ -9628,7 +9634,7 @@
       </c>
       <c r="Q16" s="24" t="str">
         <f>IF(真值表!R16=1,$O16&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="R16" s="24" t="str">
         <f>IF(真值表!S16=1,$O16&amp;"+","")</f>
@@ -9636,7 +9642,7 @@
       </c>
       <c r="S16" s="24" t="str">
         <f>IF(真值表!T16=1,$O16&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="T16" s="24" t="str">
         <f>IF(真值表!U16=1,$O16&amp;"+","")</f>
@@ -9782,7 +9788,7 @@
       </c>
       <c r="Q17" s="48" t="str">
         <f>IF(真值表!R17=1,$O17&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="R17" s="48" t="str">
         <f>IF(真值表!S17=1,$O17&amp;"+","")</f>
@@ -9790,7 +9796,7 @@
       </c>
       <c r="S17" s="48" t="str">
         <f>IF(真值表!T17=1,$O17&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="T17" s="48" t="str">
         <f>IF(真值表!U17=1,$O17&amp;"+","")</f>
@@ -11476,7 +11482,7 @@
       </c>
       <c r="Q28" s="24" t="str">
         <f>IF(真值表!R28=1,$O28&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="R28" s="24" t="str">
         <f>IF(真值表!S28=1,$O28&amp;"+","")</f>
@@ -11484,7 +11490,7 @@
       </c>
       <c r="S28" s="24" t="str">
         <f>IF(真值表!T28=1,$O28&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="T28" s="24" t="str">
         <f>IF(真值表!U28=1,$O28&amp;"+","")</f>
@@ -16053,7 +16059,7 @@
       </c>
       <c r="Q58" s="29" t="str">
         <f t="shared" si="2"/>
-        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F14&amp;~F13&amp; F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp; F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
       </c>
       <c r="R58" s="29" t="str">
         <f t="shared" si="2"/>
@@ -16061,7 +16067,7 @@
       </c>
       <c r="S58" s="31" t="str">
         <f t="shared" si="2"/>
-        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2</v>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
       </c>
       <c r="T58" s="29" t="str">
         <f t="shared" si="2"/>
@@ -16149,7 +16155,7 @@
       <c r="Q59" t="str">
         <f>CONCATENATE(Q2,Q3,Q4,Q5,Q6,Q7,Q8,Q9,Q10,Q11,Q12,Q13,Q14,Q15,Q16,Q17,Q18,Q19,Q20,Q21,Q22,Q23,Q24,Q25,Q26,Q27,Q28,Q29,Q30,Q31,Q32,Q33,Q34,Q35,Q36,Q37,Q38,Q39,Q40,Q41,Q42,Q43,Q44,Q45,Q46,Q47,Q48,Q49,Q50,Q51,Q52,Q53,Q54,Q55,Q56,Q57,
 )</f>
-        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F14&amp;~F13&amp; F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp; F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="R59" t="str">
         <f>CONCATENATE(R2,R3,R4,R5,R6,R7,R8,R9,R10,R11,R12,R13,R14,R15,R16,R17,R18,R19,R20,R21,R22,R23,R24,R25,R26,R27,R28,R29,R30,R31,R32,R33,R34,R35,R36,R37,R38,R39,R40,R41,R42,R43,R44,R45,R46,R47,R48,R49,R50,R51,R52,R53,R54,R55,R56,R57,
@@ -16159,7 +16165,7 @@
       <c r="S59" t="str">
         <f>CONCATENATE(S2,S3,S4,S5,S6,S7,S8,S9,S10,S11,S12,S13,S14,S15,S16,S17,S18,S19,S20,S21,S22,S23,S24,S25,S26,S27,S28,S29,S30,S31,S32,S33,S34,S35,S36,S37,S38,S39,S40,S41,S42,S43,S44,S45,S46,S47,S48,S49,S50,S51,S52,S53,S54,S55,S56,S57,
 )</f>
-        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+</v>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp; F14&amp; F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F30&amp;~F25&amp;~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp;~F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp;~OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp;~OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp; F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp; OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="T59" t="str">
         <f>CONCATENATE(T2,T3,T4,T5,T6,T7,T8,T9,T10,T11,T12,T13,T14,T15,T16,T17,T18,T19,T20,T21,T22,T23,T24,T25,T26,T27,T28,T29,T30,T31,T32,T33,T34,T35,T36,T37,T38,T39,T40,T41,T42,T43,T44,T45,T46,T47,T48,T49,T50,T51,T52,T53,T54,T55,T56,T57,

</xml_diff>